<commit_message>
Add capacity bound for MGT in transport
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_AFVs_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_AFVs_Growth.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vahid\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65503EDF-1EA4-433B-9AA5-1AAA5509C8BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A34C77-5589-4085-B0C3-BAEF67613389}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="49">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>T-LGT-FCV*</t>
+  </si>
+  <si>
+    <t>T-MGT-BEV*</t>
   </si>
 </sst>
 </file>
@@ -629,7 +632,7 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -656,7 +659,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="216">
@@ -1211,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1484,8 +1486,8 @@
         <v>2050</v>
       </c>
       <c r="F14" s="15">
-        <f>F13*(1.15^32)</f>
-        <v>396.66975991020649</v>
+        <f>F13*(1.17^32)</f>
+        <v>688.72488927817881</v>
       </c>
       <c r="H14" t="s">
         <v>43</v>
@@ -1645,7 +1647,7 @@
         <v>5</v>
       </c>
       <c r="G21" s="16"/>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I21" s="16" t="s">
@@ -1713,7 +1715,7 @@
         <v>5</v>
       </c>
       <c r="G24" s="16"/>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="20" t="s">
         <v>47</v>
       </c>
       <c r="I24" s="16" t="s">
@@ -1725,11 +1727,141 @@
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
     </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25">
+        <v>2019</v>
+      </c>
+      <c r="F25">
+        <v>0.4</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26">
+        <v>2050</v>
+      </c>
+      <c r="F26" s="15">
+        <f>F25*(1.15^32)</f>
+        <v>35.026027365139647</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="H27" s="20"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="16">
+        <v>0</v>
+      </c>
+      <c r="F27" s="16">
+        <v>5</v>
+      </c>
+      <c r="G27" s="16"/>
+      <c r="H27" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="H28" s="20"/>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28">
+        <v>2019</v>
+      </c>
+      <c r="F28">
+        <v>0.4</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29">
+        <v>2050</v>
+      </c>
+      <c r="F29" s="15">
+        <f>F28*(1.15^32)</f>
+        <v>35.026027365139647</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="16">
+        <v>0</v>
+      </c>
+      <c r="F30" s="16">
+        <v>5</v>
+      </c>
+      <c r="G30" s="16"/>
+      <c r="H30" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>